<commit_message>
Updated fee to 50cents and modified product backlog
</commit_message>
<xml_diff>
--- a/Homework 10/Product Backlog.xlsx
+++ b/Homework 10/Product Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atafoabure/Desktop/aaa2575_HW9/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atafoabure/Desktop/aaa2575_HW10/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{35187BA0-3601-084A-A2D4-E79A4772A9F5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A62AF9E0-7185-4045-B912-6BA3378B0279}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="181">
   <si>
     <t>Product Name:</t>
   </si>
@@ -570,9 +570,6 @@
   </si>
   <si>
     <t xml:space="preserve">Test Save and Load functionality </t>
-  </si>
-  <si>
-    <t>S</t>
   </si>
   <si>
     <t>Need to fix check in and check out for transaction</t>
@@ -801,16 +798,16 @@
                   <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1683,10 +1680,10 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2101,28 +2098,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7135,8 +7132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -7246,15 +7243,15 @@
       </c>
       <c r="B10">
         <f>C9-D10</f>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C10" s="4">
         <f>COUNT(B21:B105)</f>
         <v>28</v>
       </c>
       <c r="D10" s="4">
-        <f>D9+4</f>
-        <v>8</v>
+        <f>D9+4+2</f>
+        <v>10</v>
       </c>
       <c r="E10" s="6">
         <v>43198</v>
@@ -7266,7 +7263,7 @@
       </c>
       <c r="B11">
         <f>C10-D11</f>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C11" s="4">
         <f>COUNT(B21:B106)</f>
@@ -7274,7 +7271,7 @@
       </c>
       <c r="D11" s="4">
         <f>D10</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E11" s="6">
         <v>43205</v>
@@ -7286,7 +7283,7 @@
       </c>
       <c r="B12">
         <f>C11-D12</f>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C12" s="4">
         <f>COUNT(B21:B107)</f>
@@ -7294,7 +7291,7 @@
       </c>
       <c r="D12" s="4">
         <f>D11</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E12" s="6">
         <v>43212</v>
@@ -7306,7 +7303,7 @@
       </c>
       <c r="B13">
         <f>C12-D13</f>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C13" s="4">
         <f>COUNT(B21:B108)</f>
@@ -7314,7 +7311,7 @@
       </c>
       <c r="D13" s="4">
         <f>D12</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E13" s="6">
         <v>43219</v>
@@ -7569,11 +7566,14 @@
         <v>7</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>180</v>
+        <v>157</v>
       </c>
       <c r="D27" s="4">
         <v>2</v>
       </c>
+      <c r="E27" s="4">
+        <v>2</v>
+      </c>
       <c r="F27" t="s">
         <v>35</v>
       </c>
@@ -7590,7 +7590,7 @@
         <v>93</v>
       </c>
       <c r="K27" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -7599,9 +7599,12 @@
         <v>8</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>180</v>
+        <v>157</v>
       </c>
       <c r="D28" s="4">
+        <v>2</v>
+      </c>
+      <c r="E28" s="4">
         <v>2</v>
       </c>
       <c r="F28" t="s">
@@ -9040,8 +9043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView zoomScale="113" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -9135,8 +9138,8 @@
         <v>49</v>
       </c>
       <c r="B11" s="1">
-        <f>B10 -1</f>
-        <v>2</v>
+        <f>B10 -3</f>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -9144,8 +9147,8 @@
         <v>50</v>
       </c>
       <c r="B12" s="1">
-        <f t="shared" ref="B9:B12" si="0">B11</f>
-        <v>2</v>
+        <f t="shared" ref="B12" si="0">B11</f>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -9842,7 +9845,7 @@
         <v>177</v>
       </c>
       <c r="G45" t="s">
-        <v>28</v>
+        <v>157</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -9914,7 +9917,7 @@
         <v>139</v>
       </c>
       <c r="G48" t="s">
-        <v>28</v>
+        <v>157</v>
       </c>
       <c r="H48" t="s">
         <v>178</v>
@@ -9929,10 +9932,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -9970,7 +9973,7 @@
       </c>
       <c r="B5">
         <f>COUNT(A15:A1000)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -9979,7 +9982,7 @@
       </c>
       <c r="B6" s="1">
         <f t="shared" ref="B6:B12" si="0">B5</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -9988,7 +9991,7 @@
       </c>
       <c r="B7" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -9997,7 +10000,7 @@
       </c>
       <c r="B8" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -10006,7 +10009,7 @@
       </c>
       <c r="B9" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -10015,7 +10018,7 @@
       </c>
       <c r="B10" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -10024,7 +10027,7 @@
       </c>
       <c r="B11" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -10033,7 +10036,7 @@
       </c>
       <c r="B12" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -10060,6 +10063,28 @@
       </c>
       <c r="H17" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19">
+        <f>A18+1</f>
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="B20" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>